<commit_message>
updating to remove studies that had different means from the fluctuating and constant treatments
</commit_message>
<xml_diff>
--- a/excludeddata_14march.xlsx
+++ b/excludeddata_14march.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1418B367-8871-5544-9EC8-0C76CD29F04E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040A7E17-95B2-6543-AA29-7C27556E553A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29680" yWindow="-6800" windowWidth="23120" windowHeight="15460" xr2:uid="{1D94ADF6-B785-974B-BAAC-3A422A96ECD2}"/>
+    <workbookView xWindow="29680" yWindow="-6800" windowWidth="23120" windowHeight="15460" activeTab="1" xr2:uid="{1D94ADF6-B785-974B-BAAC-3A422A96ECD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="84">
   <si>
     <t>kern_2015phys</t>
   </si>
@@ -200,6 +201,84 @@
   <si>
     <t xml:space="preserve">figure 1d </t>
   </si>
+  <si>
+    <t>piccau2017</t>
+  </si>
+  <si>
+    <t>figure 1</t>
+  </si>
+  <si>
+    <t>germination</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>Clematis</t>
+  </si>
+  <si>
+    <t>vitalba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">irradiance per day </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 hours </t>
+  </si>
+  <si>
+    <t>duncan2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phage density </t>
+  </si>
+  <si>
+    <t>ml^-1</t>
+  </si>
+  <si>
+    <t>lytic phage</t>
+  </si>
+  <si>
+    <t>SBWΦ2.</t>
+  </si>
+  <si>
+    <t>direction of temp change</t>
+  </si>
+  <si>
+    <t>cold to hot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hot to cold </t>
+  </si>
+  <si>
+    <t>saxon2017</t>
+  </si>
+  <si>
+    <t>wing centroid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drosophila </t>
+  </si>
+  <si>
+    <t>birchii</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>different means for constant and fluctuating treatments</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>exposed to different temperatures from the experiment assay for response</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiple time points </t>
+  </si>
 </sst>
 </file>
 
@@ -214,12 +293,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -234,9 +325,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,650 +644,650 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1019FBED-5882-294F-8C12-AE6AC4298203}">
-  <dimension ref="A1:AJ108"/>
+  <dimension ref="A1:AJ114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108:XFD108"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="I1">
-        <v>24</v>
-      </c>
-      <c r="J1">
+    <row r="1" spans="1:36" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3">
         <v>20</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="3">
         <v>30</v>
       </c>
-      <c r="L1">
-        <f>K1-J1</f>
+      <c r="L1" s="3">
+        <f t="shared" ref="L1:L32" si="0">K1-J1</f>
         <v>10</v>
       </c>
-      <c r="M1">
-        <v>24</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="M1" s="3">
+        <v>24</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="3">
         <v>39.721402930000004</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="3">
         <v>40.514995859999999</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="3">
         <v>7.5117371000000002E-2</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="3">
         <v>0.16901408500000001</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="3">
         <v>192</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="3">
         <v>192</v>
       </c>
-      <c r="V1">
-        <v>1</v>
-      </c>
-      <c r="W1">
-        <v>0</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="V1" s="3">
+        <v>1</v>
+      </c>
+      <c r="W1" s="3">
+        <v>0</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Z1">
-        <v>1</v>
-      </c>
-      <c r="AA1">
-        <v>1</v>
-      </c>
-      <c r="AB1">
-        <v>2</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="Z1" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>2</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="2" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>24</v>
-      </c>
-      <c r="J2">
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3">
         <v>20</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>30</v>
       </c>
-      <c r="L2">
-        <f>K2-J2</f>
+      <c r="L2" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M2">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="M2" s="3">
+        <v>24</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="3">
         <v>40.488262910000003</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="3">
         <v>41.57722708</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="3">
         <v>0.112676056</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="3">
         <v>9.3896714000000006E-2</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="3">
         <v>163</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="3">
         <v>163</v>
       </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="V2" s="3">
+        <v>1</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z2">
-        <v>1</v>
-      </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>2</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="Z2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="3" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>24</v>
-      </c>
-      <c r="J3">
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3">
         <v>20</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>30</v>
       </c>
-      <c r="L3">
-        <f>K3-J3</f>
+      <c r="L3" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M3">
-        <v>24</v>
-      </c>
-      <c r="N3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="M3" s="3">
+        <v>24</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="3">
         <v>41.73584906</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="3">
         <v>42.90566038</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="3">
         <v>0.15094339600000001</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="3">
         <v>0.132075472</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="3">
         <v>245</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="3">
         <v>245</v>
       </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="V3" s="3">
+        <v>1</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Z3">
-        <v>1</v>
-      </c>
-      <c r="AA3">
-        <v>1</v>
-      </c>
-      <c r="AB3">
-        <v>2</v>
-      </c>
-      <c r="AJ3" t="s">
+      <c r="Z3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="4" spans="1:36" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="I4">
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
         <v>18</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>18</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>28</v>
       </c>
-      <c r="L4">
-        <f>K4-J4</f>
+      <c r="L4" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M4">
-        <v>24</v>
-      </c>
-      <c r="N4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="M4" s="3">
+        <v>24</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="3">
         <v>39.8815144</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="3">
         <v>40.29342261</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="3">
         <v>0.13501144000000001</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="3">
         <v>6.8649885999999993E-2</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="3">
         <v>12</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="3">
         <v>12</v>
       </c>
-      <c r="V4">
-        <v>1</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="V4" s="3">
+        <v>1</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Y4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Z4">
-        <v>1</v>
-      </c>
-      <c r="AA4">
-        <v>1</v>
-      </c>
-      <c r="AB4">
-        <v>2</v>
-      </c>
-      <c r="AC4" t="s">
+      <c r="Z4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AD4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="5" spans="1:36" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="I5">
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
         <v>18</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <v>18</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <v>28</v>
       </c>
-      <c r="L5">
-        <f>K5-J5</f>
+      <c r="L5" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M5">
-        <v>24</v>
-      </c>
-      <c r="N5" t="s">
-        <v>2</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="M5" s="3">
+        <v>24</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="3">
         <v>39.947047900000001</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="3">
         <v>40.432164829999998</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="3">
         <v>0.13043478</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="3">
         <v>0.11442537999999999</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="3">
         <v>12</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="3">
         <v>12</v>
       </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="V5" s="3">
+        <v>1</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0</v>
+      </c>
+      <c r="X5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Y5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Z5">
-        <v>1</v>
-      </c>
-      <c r="AA5">
-        <v>1</v>
-      </c>
-      <c r="AB5">
-        <v>2</v>
-      </c>
-      <c r="AC5" t="s">
+      <c r="Z5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AD5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AJ5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="6" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>24</v>
-      </c>
-      <c r="I6">
-        <v>24</v>
-      </c>
-      <c r="J6">
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>24</v>
+      </c>
+      <c r="I6" s="3">
+        <v>24</v>
+      </c>
+      <c r="J6" s="3">
         <v>18</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <v>32</v>
       </c>
-      <c r="L6">
-        <f>K6-J6</f>
+      <c r="L6" s="3">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="M6">
-        <v>24</v>
-      </c>
-      <c r="N6" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="M6" s="3">
+        <v>24</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="3">
         <v>42.15384615</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="3">
         <v>42.335664340000001</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="3">
         <v>0.125874126</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="3">
         <v>0.12937062899999999</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="3">
         <v>8</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="3">
         <v>8</v>
       </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="V6" s="3">
+        <v>1</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0</v>
+      </c>
+      <c r="X6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Y6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Z6">
-        <v>1</v>
-      </c>
-      <c r="AA6">
-        <v>1</v>
-      </c>
-      <c r="AB6">
-        <v>2</v>
-      </c>
-      <c r="AC6" t="s">
+      <c r="Z6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AJ6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="7" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>24</v>
-      </c>
-      <c r="I7">
-        <v>24</v>
-      </c>
-      <c r="J7">
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>24</v>
+      </c>
+      <c r="I7" s="3">
+        <v>24</v>
+      </c>
+      <c r="J7" s="3">
         <v>18</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <v>32</v>
       </c>
-      <c r="L7">
-        <f>K7-J7</f>
+      <c r="L7" s="3">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="M7">
-        <v>24</v>
-      </c>
-      <c r="N7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="M7" s="3">
+        <v>24</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="3">
         <v>41.398601399999997</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="3">
         <v>43.006993010000002</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="3">
         <v>0.12237762200000001</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="3">
         <v>0.19580419600000001</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="3">
         <v>8</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="3">
         <v>8</v>
       </c>
-      <c r="V7">
-        <v>1</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7" t="s">
+      <c r="V7" s="3">
+        <v>1</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Y7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Z7">
-        <v>1</v>
-      </c>
-      <c r="AA7">
-        <v>1</v>
-      </c>
-      <c r="AB7">
-        <v>2</v>
-      </c>
-      <c r="AC7" t="s">
+      <c r="Z7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AD7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AJ7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1230,7 +1323,7 @@
         <v>31</v>
       </c>
       <c r="L8">
-        <f>K8-J8</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M8">
@@ -1329,7 +1422,7 @@
         <v>31</v>
       </c>
       <c r="L9">
-        <f>K9-J9</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M9">
@@ -1428,7 +1521,7 @@
         <v>31</v>
       </c>
       <c r="L10">
-        <f>K10-J10</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M10">
@@ -1527,7 +1620,7 @@
         <v>31</v>
       </c>
       <c r="L11">
-        <f>K11-J11</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M11">
@@ -1626,7 +1719,7 @@
         <v>31</v>
       </c>
       <c r="L12">
-        <f>K12-J12</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M12">
@@ -1719,7 +1812,7 @@
         <v>34</v>
       </c>
       <c r="L13">
-        <f>K13-J13</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M13">
@@ -1818,7 +1911,7 @@
         <v>34</v>
       </c>
       <c r="L14">
-        <f>K14-J14</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M14">
@@ -1917,7 +2010,7 @@
         <v>34</v>
       </c>
       <c r="L15">
-        <f>K15-J15</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M15">
@@ -2016,7 +2109,7 @@
         <v>34</v>
       </c>
       <c r="L16">
-        <f>K16-J16</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M16">
@@ -2115,7 +2208,7 @@
         <v>34</v>
       </c>
       <c r="L17">
-        <f>K17-J17</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M17">
@@ -2208,7 +2301,7 @@
         <v>31</v>
       </c>
       <c r="L18">
-        <f>K18-J18</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M18">
@@ -2307,7 +2400,7 @@
         <v>31</v>
       </c>
       <c r="L19">
-        <f>K19-J19</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M19">
@@ -2406,7 +2499,7 @@
         <v>31</v>
       </c>
       <c r="L20">
-        <f>K20-J20</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M20">
@@ -2505,7 +2598,7 @@
         <v>31</v>
       </c>
       <c r="L21">
-        <f>K21-J21</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M21">
@@ -2604,7 +2697,7 @@
         <v>31</v>
       </c>
       <c r="L22">
-        <f>K22-J22</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M22">
@@ -2697,7 +2790,7 @@
         <v>34</v>
       </c>
       <c r="L23">
-        <f>K23-J23</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M23">
@@ -2796,7 +2889,7 @@
         <v>34</v>
       </c>
       <c r="L24">
-        <f>K24-J24</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M24">
@@ -2895,7 +2988,7 @@
         <v>34</v>
       </c>
       <c r="L25">
-        <f>K25-J25</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M25">
@@ -2994,7 +3087,7 @@
         <v>34</v>
       </c>
       <c r="L26">
-        <f>K26-J26</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M26">
@@ -3093,7 +3186,7 @@
         <v>34</v>
       </c>
       <c r="L27">
-        <f>K27-J27</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M27">
@@ -3186,7 +3279,7 @@
         <v>32</v>
       </c>
       <c r="L28">
-        <f>K28-J28</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="M28">
@@ -3282,7 +3375,7 @@
         <v>32</v>
       </c>
       <c r="L29">
-        <f>K29-J29</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="M29">
@@ -3381,7 +3474,7 @@
         <v>32</v>
       </c>
       <c r="L30">
-        <f>K30-J30</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="M30">
@@ -3480,7 +3573,7 @@
         <v>32</v>
       </c>
       <c r="L31">
-        <f>K31-J31</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="M31">
@@ -3579,7 +3672,7 @@
         <v>32</v>
       </c>
       <c r="L32">
-        <f>K32-J32</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="M32">
@@ -3678,7 +3771,7 @@
         <v>32</v>
       </c>
       <c r="L33">
-        <f>K33-J33</f>
+        <f t="shared" ref="L33:L64" si="1">K33-J33</f>
         <v>15</v>
       </c>
       <c r="M33">
@@ -3777,7 +3870,7 @@
         <v>32</v>
       </c>
       <c r="L34">
-        <f>K34-J34</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M34">
@@ -3876,7 +3969,7 @@
         <v>32</v>
       </c>
       <c r="L35">
-        <f>K35-J35</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M35">
@@ -3975,7 +4068,7 @@
         <v>32</v>
       </c>
       <c r="L36">
-        <f>K36-J36</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M36">
@@ -4074,7 +4167,7 @@
         <v>32</v>
       </c>
       <c r="L37">
-        <f>K37-J37</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M37">
@@ -4173,7 +4266,7 @@
         <v>32</v>
       </c>
       <c r="L38">
-        <f>K38-J38</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M38">
@@ -4272,7 +4365,7 @@
         <v>32</v>
       </c>
       <c r="L39">
-        <f>K39-J39</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M39">
@@ -4371,7 +4464,7 @@
         <v>32</v>
       </c>
       <c r="L40">
-        <f>K40-J40</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M40">
@@ -4467,7 +4560,7 @@
         <v>32</v>
       </c>
       <c r="L41">
-        <f>K41-J41</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M41">
@@ -4560,7 +4653,7 @@
         <v>32</v>
       </c>
       <c r="L42">
-        <f>K42-J42</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M42">
@@ -4653,7 +4746,7 @@
         <v>32</v>
       </c>
       <c r="L43">
-        <f>K43-J43</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M43">
@@ -4746,7 +4839,7 @@
         <v>32</v>
       </c>
       <c r="L44">
-        <f>K44-J44</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M44">
@@ -4839,7 +4932,7 @@
         <v>32</v>
       </c>
       <c r="L45">
-        <f>K45-J45</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M45">
@@ -4935,7 +5028,7 @@
         <v>32</v>
       </c>
       <c r="L46">
-        <f>K46-J46</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M46">
@@ -5034,7 +5127,7 @@
         <v>32</v>
       </c>
       <c r="L47">
-        <f>K47-J47</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M47">
@@ -5133,7 +5226,7 @@
         <v>32</v>
       </c>
       <c r="L48">
-        <f>K48-J48</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M48">
@@ -5232,7 +5325,7 @@
         <v>32</v>
       </c>
       <c r="L49">
-        <f>K49-J49</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M49">
@@ -5331,7 +5424,7 @@
         <v>32</v>
       </c>
       <c r="L50">
-        <f>K50-J50</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M50">
@@ -5430,7 +5523,7 @@
         <v>32</v>
       </c>
       <c r="L51">
-        <f>K51-J51</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M51">
@@ -5529,7 +5622,7 @@
         <v>32</v>
       </c>
       <c r="L52">
-        <f>K52-J52</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M52">
@@ -5628,7 +5721,7 @@
         <v>32</v>
       </c>
       <c r="L53">
-        <f>K53-J53</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M53">
@@ -5727,7 +5820,7 @@
         <v>32</v>
       </c>
       <c r="L54">
-        <f>K54-J54</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M54">
@@ -5820,7 +5913,7 @@
         <v>32</v>
       </c>
       <c r="L55">
-        <f>K55-J55</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M55">
@@ -5913,7 +6006,7 @@
         <v>32</v>
       </c>
       <c r="L56">
-        <f>K56-J56</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M56">
@@ -6009,7 +6102,7 @@
         <v>32</v>
       </c>
       <c r="L57">
-        <f>K57-J57</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M57">
@@ -6108,7 +6201,7 @@
         <v>32</v>
       </c>
       <c r="L58">
-        <f>K58-J58</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M58">
@@ -6207,7 +6300,7 @@
         <v>32</v>
       </c>
       <c r="L59">
-        <f>K59-J59</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M59">
@@ -6306,7 +6399,7 @@
         <v>32</v>
       </c>
       <c r="L60">
-        <f>K60-J60</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M60">
@@ -6405,7 +6498,7 @@
         <v>32</v>
       </c>
       <c r="L61">
-        <f>K61-J61</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M61">
@@ -6504,7 +6597,7 @@
         <v>32</v>
       </c>
       <c r="L62">
-        <f>K62-J62</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M62">
@@ -6603,7 +6696,7 @@
         <v>32</v>
       </c>
       <c r="L63">
-        <f>K63-J63</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M63">
@@ -6702,7 +6795,7 @@
         <v>32</v>
       </c>
       <c r="L64">
-        <f>K64-J64</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M64">
@@ -6801,7 +6894,7 @@
         <v>32</v>
       </c>
       <c r="L65">
-        <f>K65-J65</f>
+        <f t="shared" ref="L65:L96" si="2">K65-J65</f>
         <v>15</v>
       </c>
       <c r="M65">
@@ -6900,7 +6993,7 @@
         <v>32</v>
       </c>
       <c r="L66">
-        <f>K66-J66</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M66">
@@ -6999,7 +7092,7 @@
         <v>32</v>
       </c>
       <c r="L67">
-        <f>K67-J67</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M67">
@@ -7092,7 +7185,7 @@
         <v>32</v>
       </c>
       <c r="L68">
-        <f>K68-J68</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M68">
@@ -7185,7 +7278,7 @@
         <v>32</v>
       </c>
       <c r="L69">
-        <f>K69-J69</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M69">
@@ -7278,7 +7371,7 @@
         <v>32</v>
       </c>
       <c r="L70">
-        <f>K70-J70</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M70">
@@ -7371,7 +7464,7 @@
         <v>32</v>
       </c>
       <c r="L71">
-        <f>K71-J71</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M71">
@@ -7464,7 +7557,7 @@
         <v>32</v>
       </c>
       <c r="L72">
-        <f>K72-J72</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M72">
@@ -7560,7 +7653,7 @@
         <v>32</v>
       </c>
       <c r="L73">
-        <f>K73-J73</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M73">
@@ -7659,7 +7752,7 @@
         <v>32</v>
       </c>
       <c r="L74">
-        <f>K74-J74</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M74">
@@ -7758,7 +7851,7 @@
         <v>32</v>
       </c>
       <c r="L75">
-        <f>K75-J75</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M75">
@@ -7857,7 +7950,7 @@
         <v>32</v>
       </c>
       <c r="L76">
-        <f>K76-J76</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M76">
@@ -7956,7 +8049,7 @@
         <v>32</v>
       </c>
       <c r="L77">
-        <f>K77-J77</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M77">
@@ -8055,7 +8148,7 @@
         <v>32</v>
       </c>
       <c r="L78">
-        <f>K78-J78</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M78">
@@ -8154,7 +8247,7 @@
         <v>32</v>
       </c>
       <c r="L79">
-        <f>K79-J79</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M79">
@@ -8256,7 +8349,7 @@
         <v>14</v>
       </c>
       <c r="L80">
-        <f>K80-J80</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M80">
@@ -8355,7 +8448,7 @@
         <v>14</v>
       </c>
       <c r="L81">
-        <f>K81-J81</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M81">
@@ -8451,7 +8544,7 @@
         <v>23</v>
       </c>
       <c r="L82">
-        <f>K82-J82</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M82">
@@ -8553,7 +8646,7 @@
         <v>23</v>
       </c>
       <c r="L83">
-        <f>K83-J83</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M83">
@@ -8649,7 +8742,7 @@
         <v>30</v>
       </c>
       <c r="L84">
-        <f>K84-J84</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M84">
@@ -8748,7 +8841,7 @@
         <v>30</v>
       </c>
       <c r="L85">
-        <f>K85-J85</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M85">
@@ -8847,7 +8940,7 @@
         <v>14</v>
       </c>
       <c r="L86">
-        <f>K86-J86</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M86">
@@ -8946,7 +9039,7 @@
         <v>14</v>
       </c>
       <c r="L87">
-        <f>K87-J87</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M87">
@@ -9042,7 +9135,7 @@
         <v>23</v>
       </c>
       <c r="L88">
-        <f>K88-J88</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M88">
@@ -9144,7 +9237,7 @@
         <v>23</v>
       </c>
       <c r="L89">
-        <f>K89-J89</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M89">
@@ -9240,7 +9333,7 @@
         <v>30</v>
       </c>
       <c r="L90">
-        <f>K90-J90</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M90">
@@ -9342,7 +9435,7 @@
         <v>30</v>
       </c>
       <c r="L91">
-        <f>K91-J91</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M91">
@@ -9438,7 +9531,7 @@
         <v>40</v>
       </c>
       <c r="L92">
-        <f>K92-J92</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M92">
@@ -9534,7 +9627,7 @@
         <v>14</v>
       </c>
       <c r="L93">
-        <f>K93-J93</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M93">
@@ -9633,7 +9726,7 @@
         <v>14</v>
       </c>
       <c r="L94">
-        <f>K94-J94</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M94">
@@ -9732,7 +9825,7 @@
         <v>23</v>
       </c>
       <c r="L95">
-        <f>K95-J95</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M95">
@@ -9834,7 +9927,7 @@
         <v>23</v>
       </c>
       <c r="L96">
-        <f>K96-J96</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M96">
@@ -9930,7 +10023,7 @@
         <v>30</v>
       </c>
       <c r="L97">
-        <f>K97-J97</f>
+        <f t="shared" ref="L97:L108" si="3">K97-J97</f>
         <v>14</v>
       </c>
       <c r="M97">
@@ -10032,7 +10125,7 @@
         <v>30</v>
       </c>
       <c r="L98">
-        <f>K98-J98</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M98">
@@ -10128,7 +10221,7 @@
         <v>40</v>
       </c>
       <c r="L99">
-        <f>K99-J99</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M99">
@@ -10230,7 +10323,7 @@
         <v>40</v>
       </c>
       <c r="L100">
-        <f>K100-J100</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M100">
@@ -10326,7 +10419,7 @@
         <v>14</v>
       </c>
       <c r="L101">
-        <f>K101-J101</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M101">
@@ -10429,7 +10522,7 @@
         <v>14</v>
       </c>
       <c r="L102">
-        <f>K102-J102</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M102">
@@ -10526,7 +10619,7 @@
         <v>23</v>
       </c>
       <c r="L103">
-        <f>K103-J103</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M103">
@@ -10626,7 +10719,7 @@
         <v>23</v>
       </c>
       <c r="L104">
-        <f>K104-J104</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M104">
@@ -10723,7 +10816,7 @@
         <v>30</v>
       </c>
       <c r="L105">
-        <f>K105-J105</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M105">
@@ -10823,7 +10916,7 @@
         <v>30</v>
       </c>
       <c r="L106">
-        <f>K106-J106</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M106">
@@ -10920,7 +11013,7 @@
         <v>40</v>
       </c>
       <c r="L107">
-        <f>K107-J107</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M107">
@@ -11020,7 +11113,7 @@
         <v>40</v>
       </c>
       <c r="L108">
-        <f>K108-J108</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M108">
@@ -11080,6 +11173,588 @@
       </c>
       <c r="AJ108" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2">
+        <v>1</v>
+      </c>
+      <c r="B109" s="2">
+        <v>1</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E109" s="2">
+        <v>1</v>
+      </c>
+      <c r="F109" s="2">
+        <v>1</v>
+      </c>
+      <c r="G109" s="2">
+        <v>1</v>
+      </c>
+      <c r="I109" s="2">
+        <v>10</v>
+      </c>
+      <c r="J109" s="2">
+        <v>10</v>
+      </c>
+      <c r="K109" s="2">
+        <v>25</v>
+      </c>
+      <c r="L109" s="2">
+        <f>K109-J109</f>
+        <v>15</v>
+      </c>
+      <c r="M109" s="2">
+        <v>24</v>
+      </c>
+      <c r="N109" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O109" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P109" s="2">
+        <v>0.81037276999999996</v>
+      </c>
+      <c r="Q109" s="2">
+        <v>87.520259300000006</v>
+      </c>
+      <c r="R109" s="2">
+        <v>1.6207455399999999</v>
+      </c>
+      <c r="S109" s="2">
+        <v>7.3743922199999998</v>
+      </c>
+      <c r="T109" s="2">
+        <v>120</v>
+      </c>
+      <c r="U109" s="2">
+        <v>120</v>
+      </c>
+      <c r="V109" s="2">
+        <v>1</v>
+      </c>
+      <c r="W109" s="2">
+        <v>1</v>
+      </c>
+      <c r="X109" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y109" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z109" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA109" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB109" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC109" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD109" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ109" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="110" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="2">
+        <v>1</v>
+      </c>
+      <c r="B110" s="2">
+        <v>1</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E110" s="2">
+        <v>0</v>
+      </c>
+      <c r="F110" s="2">
+        <v>4</v>
+      </c>
+      <c r="G110" s="2">
+        <v>0</v>
+      </c>
+      <c r="I110" s="2">
+        <v>32</v>
+      </c>
+      <c r="J110" s="2">
+        <v>28</v>
+      </c>
+      <c r="K110" s="2">
+        <v>32</v>
+      </c>
+      <c r="L110" s="2">
+        <f>K110-J110</f>
+        <v>4</v>
+      </c>
+      <c r="M110" s="2">
+        <v>48</v>
+      </c>
+      <c r="N110" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O110" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P110" s="2">
+        <v>-2.3909825023451015E-2</v>
+      </c>
+      <c r="Q110" s="2">
+        <v>-0.84509945900000005</v>
+      </c>
+      <c r="R110" s="2">
+        <v>0.11820634261581375</v>
+      </c>
+      <c r="S110" s="2">
+        <v>0.119565036</v>
+      </c>
+      <c r="V110" s="2">
+        <v>1</v>
+      </c>
+      <c r="W110" s="2">
+        <v>0</v>
+      </c>
+      <c r="X110" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y110" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z110" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA110" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB110" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC110" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD110" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ110" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="2">
+        <v>1</v>
+      </c>
+      <c r="B111" s="2">
+        <v>2</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E111" s="2">
+        <v>0</v>
+      </c>
+      <c r="F111" s="2">
+        <v>4</v>
+      </c>
+      <c r="G111" s="2">
+        <v>0</v>
+      </c>
+      <c r="I111" s="2">
+        <v>32</v>
+      </c>
+      <c r="J111" s="2">
+        <v>28</v>
+      </c>
+      <c r="K111" s="2">
+        <v>32</v>
+      </c>
+      <c r="L111" s="2">
+        <f>K111-J111</f>
+        <v>4</v>
+      </c>
+      <c r="M111" s="2">
+        <v>48</v>
+      </c>
+      <c r="N111" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O111" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P111" s="2">
+        <v>-2.3909825023451015E-2</v>
+      </c>
+      <c r="Q111" s="2">
+        <v>2.4135967100000002</v>
+      </c>
+      <c r="R111" s="2">
+        <v>0.11820634261581375</v>
+      </c>
+      <c r="S111" s="2">
+        <v>0.28260826700000002</v>
+      </c>
+      <c r="V111" s="2">
+        <v>1</v>
+      </c>
+      <c r="W111" s="2">
+        <v>0</v>
+      </c>
+      <c r="X111" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y111" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z111" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA111" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB111" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC111" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD111" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ111" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="112" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="2">
+        <v>3</v>
+      </c>
+      <c r="B112" s="2">
+        <v>3</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E112" s="2">
+        <v>0</v>
+      </c>
+      <c r="F112" s="2">
+        <v>1</v>
+      </c>
+      <c r="G112" s="2">
+        <v>1</v>
+      </c>
+      <c r="H112" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="I112" s="2">
+        <v>21</v>
+      </c>
+      <c r="J112" s="2">
+        <v>21</v>
+      </c>
+      <c r="K112" s="2">
+        <v>27</v>
+      </c>
+      <c r="L112" s="2">
+        <f>K112-J112</f>
+        <v>6</v>
+      </c>
+      <c r="M112" s="2">
+        <v>24</v>
+      </c>
+      <c r="N112" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O112" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P112" s="2">
+        <v>2089.0710382513648</v>
+      </c>
+      <c r="Q112" s="2">
+        <v>2006.010929</v>
+      </c>
+      <c r="R112" s="2">
+        <v>74.478850435137048</v>
+      </c>
+      <c r="S112" s="2">
+        <v>74.478850440000002</v>
+      </c>
+      <c r="T112" s="2">
+        <v>480</v>
+      </c>
+      <c r="U112" s="2">
+        <v>480</v>
+      </c>
+      <c r="V112" s="2">
+        <v>1</v>
+      </c>
+      <c r="W112" s="2">
+        <v>1</v>
+      </c>
+      <c r="X112" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y112" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z112" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA112" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB112" s="2">
+        <v>1</v>
+      </c>
+      <c r="AJ112" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:36" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
+        <v>1</v>
+      </c>
+      <c r="B113" s="2">
+        <v>1</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E113" s="2">
+        <v>1</v>
+      </c>
+      <c r="F113" s="2">
+        <v>1</v>
+      </c>
+      <c r="G113" s="2">
+        <v>1</v>
+      </c>
+      <c r="I113" s="2">
+        <v>18</v>
+      </c>
+      <c r="J113" s="2">
+        <v>18</v>
+      </c>
+      <c r="K113" s="2">
+        <v>28</v>
+      </c>
+      <c r="L113" s="2">
+        <f>K113-J113</f>
+        <v>10</v>
+      </c>
+      <c r="M113" s="2">
+        <v>24</v>
+      </c>
+      <c r="N113" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O113" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P113" s="2">
+        <v>86.5139949</v>
+      </c>
+      <c r="Q113" s="2">
+        <v>83.460559799999999</v>
+      </c>
+      <c r="R113" s="2">
+        <v>3.1170483449999997</v>
+      </c>
+      <c r="S113" s="2">
+        <v>6.361323155</v>
+      </c>
+      <c r="T113" s="2">
+        <v>12</v>
+      </c>
+      <c r="U113" s="2">
+        <v>12</v>
+      </c>
+      <c r="V113" s="2">
+        <v>1</v>
+      </c>
+      <c r="W113" s="2">
+        <v>0</v>
+      </c>
+      <c r="X113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y113" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z113" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA113" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB113" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC113" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD113" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ113" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="114" spans="1:36" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>1</v>
+      </c>
+      <c r="B114" s="2">
+        <v>1</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E114" s="2">
+        <v>1</v>
+      </c>
+      <c r="F114" s="2">
+        <v>1</v>
+      </c>
+      <c r="G114" s="2">
+        <v>1</v>
+      </c>
+      <c r="I114" s="2">
+        <v>18</v>
+      </c>
+      <c r="J114" s="2">
+        <v>18</v>
+      </c>
+      <c r="K114" s="2">
+        <v>28</v>
+      </c>
+      <c r="L114" s="2">
+        <f>K114-J114</f>
+        <v>10</v>
+      </c>
+      <c r="M114" s="2">
+        <v>24</v>
+      </c>
+      <c r="N114" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O114" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P114" s="2">
+        <v>21.628498699999994</v>
+      </c>
+      <c r="Q114" s="2">
+        <v>80.91603053</v>
+      </c>
+      <c r="R114" s="2">
+        <v>6.4885496200000006</v>
+      </c>
+      <c r="S114" s="2">
+        <v>6.9974554710000003</v>
+      </c>
+      <c r="T114" s="2">
+        <v>12</v>
+      </c>
+      <c r="U114" s="2">
+        <v>12</v>
+      </c>
+      <c r="V114" s="2">
+        <v>1</v>
+      </c>
+      <c r="W114" s="2">
+        <v>0</v>
+      </c>
+      <c r="X114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y114" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z114" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA114" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB114" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC114" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD114" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ114" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{763313DD-8534-5C4C-8D9C-F3CA4E15A34E}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>